<commit_message>
typo and minor change
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Metro_System_Data.xlsx
+++ b/src/main/resources/Data/Metro_System_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikas\IdeaProjects\MetroRoutePredictor\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D6AE2-3309-4921-88F9-F9F085251748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED47B1D-9BAB-4A4B-8199-A91E92A84856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2BA787B-7146-4090-B2DF-9614BCEDDEDC}"/>
+    <workbookView xWindow="2520" yWindow="2496" windowWidth="17280" windowHeight="9420" xr2:uid="{C2BA787B-7146-4090-B2DF-9614BCEDDEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="266">
   <si>
     <t>stations</t>
   </si>
@@ -942,98 +942,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1353,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A42BA0A-D4BB-482D-AE39-D8364F7AF299}">
   <dimension ref="A1:J492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2645,13 +2554,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B44">
-        <v>28.643721680018999</v>
+        <v>28.623350504979499</v>
       </c>
       <c r="C44">
-        <v>77.222991097534702</v>
+        <v>77.214508120105805</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>23</v>
@@ -2675,13 +2584,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B45">
-        <v>28.623350504979499</v>
+        <v>28.6151513673286</v>
       </c>
       <c r="C45">
-        <v>77.214508120105805</v>
+        <v>77.212263415491904</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>24</v>
@@ -2705,13 +2614,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B46">
-        <v>28.6151513673286</v>
+        <v>28.610709339302002</v>
       </c>
       <c r="C46">
-        <v>77.212263415491904</v>
+        <v>77.211881866970998</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>25</v>
@@ -2735,13 +2644,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47">
-        <v>28.610709339302002</v>
+        <v>28.5976559905465</v>
       </c>
       <c r="C47">
-        <v>77.211881866970998</v>
+        <v>77.2111753147569</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>26</v>
@@ -2765,13 +2674,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B48">
-        <v>28.5976559905465</v>
+        <v>28.585887691418201</v>
       </c>
       <c r="C48">
-        <v>77.2111753147569</v>
+        <v>77.212510728205899</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>27</v>
@@ -2795,13 +2704,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B49">
-        <v>28.585887691418201</v>
+        <v>28.5744485641743</v>
       </c>
       <c r="C49">
-        <v>77.212510728205899</v>
+        <v>77.209623783504199</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>28</v>
@@ -2825,13 +2734,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50">
-        <v>28.5744485641743</v>
+        <v>28.567800555611701</v>
       </c>
       <c r="C50">
-        <v>77.209623783504199</v>
+        <v>77.207759982508904</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>29</v>
@@ -2855,13 +2764,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51">
-        <v>28.567800555611701</v>
+        <v>28.559820911682799</v>
       </c>
       <c r="C51">
-        <v>77.207759982508904</v>
+        <v>77.206829850808305</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>30</v>
@@ -2885,13 +2794,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <v>28.559820911682799</v>
+        <v>28.543949735241899</v>
       </c>
       <c r="C52">
-        <v>77.206829850808305</v>
+        <v>77.2062402425382</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>31</v>
@@ -2915,13 +2824,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <v>28.543949735241899</v>
+        <v>28.528988096353299</v>
       </c>
       <c r="C53">
-        <v>77.2062402425382</v>
+        <v>77.204991220641006</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>32</v>
@@ -2945,13 +2854,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B54">
-        <v>28.528988096353299</v>
+        <v>28.521130210440599</v>
       </c>
       <c r="C54">
-        <v>77.204991220641006</v>
+        <v>77.202180427118805</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>33</v>
@@ -2975,13 +2884,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B55">
-        <v>28.521130210440599</v>
+        <v>28.513019785996001</v>
       </c>
       <c r="C55">
-        <v>77.202180427118805</v>
+        <v>77.186400611549502</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>34</v>
@@ -3005,13 +2914,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B56">
-        <v>28.513019785996001</v>
+        <v>28.506792858417398</v>
       </c>
       <c r="C56">
-        <v>77.186400611549502</v>
+        <v>77.175026511693503</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>35</v>
@@ -3035,13 +2944,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B57">
-        <v>28.506792858417398</v>
+        <v>28.499152242649402</v>
       </c>
       <c r="C57">
-        <v>77.175026511693503</v>
+        <v>77.161536752928399</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>36</v>
@@ -3065,13 +2974,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B58">
-        <v>28.499152242649402</v>
+        <v>28.493814210798298</v>
       </c>
       <c r="C58">
-        <v>77.161536752928399</v>
+        <v>77.149174853487906</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>37</v>
@@ -3095,13 +3004,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B59">
-        <v>28.493814210798298</v>
+        <v>28.4808777371906</v>
       </c>
       <c r="C59">
-        <v>77.149174853487906</v>
+        <v>77.125850668097399</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>42</v>
@@ -3125,13 +3034,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B60">
-        <v>28.4808777371906</v>
+        <v>28.481949531523</v>
       </c>
       <c r="C60">
-        <v>77.125850668097399</v>
+        <v>77.102251322097501</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>43</v>
@@ -3155,13 +3064,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B61">
-        <v>28.481949531523</v>
+        <v>28.481308576797201</v>
       </c>
       <c r="C61">
-        <v>77.102251322097501</v>
+        <v>77.093118677973195</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>44</v>
@@ -3185,13 +3094,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B62">
-        <v>28.481308576797201</v>
+        <v>28.479570018235101</v>
       </c>
       <c r="C62">
-        <v>77.093118677973195</v>
+        <v>77.080060966573996</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>45</v>
@@ -3215,13 +3124,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63">
-        <v>28.479570018235101</v>
+        <v>28.472239422067801</v>
       </c>
       <c r="C63">
-        <v>77.080060966573996</v>
+        <v>77.072399591572093</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>46</v>
@@ -3245,13 +3154,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B64">
-        <v>28.472239422067801</v>
+        <v>28.459198447634201</v>
       </c>
       <c r="C64">
-        <v>77.072399591572093</v>
+        <v>77.072480927578397</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>47</v>
@@ -3274,14 +3183,14 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>77</v>
+      <c r="A65" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="B65">
-        <v>28.459198447634201</v>
+        <v>28.627941651175199</v>
       </c>
       <c r="C65">
-        <v>77.072480927578397</v>
+        <v>77.374931005109801</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>48</v>
@@ -3305,13 +3214,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B66">
-        <v>28.627941651175199</v>
+        <v>28.616996235641</v>
       </c>
       <c r="C66">
-        <v>77.374931005109801</v>
+        <v>77.373610851992893</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>49</v>
@@ -3335,13 +3244,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B67">
-        <v>28.616996235641</v>
+        <v>28.6064935182097</v>
       </c>
       <c r="C67">
-        <v>77.373610851992893</v>
+        <v>77.372723809811006</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>50</v>
@@ -3365,13 +3274,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68">
-        <v>28.6064935182097</v>
+        <v>28.597630605063198</v>
       </c>
       <c r="C68">
-        <v>77.372723809811006</v>
+        <v>77.372300481976893</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>51</v>
@@ -3395,13 +3304,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B69">
-        <v>28.597630605063198</v>
+        <v>28.5866997280344</v>
       </c>
       <c r="C69">
-        <v>77.372300481976893</v>
+        <v>77.372839101422798</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>52</v>
@@ -3425,13 +3334,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B70">
-        <v>28.5866997280344</v>
+        <v>28.580118102895099</v>
       </c>
       <c r="C70">
-        <v>77.372839101422798</v>
+        <v>77.363487259603801</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>24</v>
@@ -3455,13 +3364,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B71">
-        <v>28.580118102895099</v>
+        <v>28.5746701138224</v>
       </c>
       <c r="C71">
-        <v>77.363487259603801</v>
+        <v>77.356050762406497</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>53</v>
@@ -3485,13 +3394,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B72">
-        <v>28.5746701138224</v>
+        <v>28.567190661055399</v>
       </c>
       <c r="C72">
-        <v>77.356050762406497</v>
+        <v>77.3459713962162</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>54</v>
@@ -3515,13 +3424,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B73">
-        <v>28.567190661055399</v>
+        <v>28.564031310067801</v>
       </c>
       <c r="C73">
-        <v>77.3459713962162</v>
+        <v>77.334281259654105</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>55</v>
@@ -3545,13 +3454,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B74">
-        <v>28.564031310067801</v>
+        <v>28.570749578225598</v>
       </c>
       <c r="C74">
-        <v>77.334281259654105</v>
+        <v>77.3261861280061</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>56</v>
@@ -3575,13 +3484,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B75">
-        <v>28.570749578225598</v>
+        <v>28.578235360780202</v>
       </c>
       <c r="C75">
-        <v>77.3261861280061</v>
+        <v>77.317721267357001</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>57</v>
@@ -3605,13 +3514,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B76">
-        <v>28.578235360780202</v>
+        <v>28.5850880881497</v>
       </c>
       <c r="C76">
-        <v>77.317721267357001</v>
+        <v>77.311591878090894</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>58</v>
@@ -3635,13 +3544,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B77">
-        <v>28.5850880881497</v>
+        <v>28.589156773171101</v>
       </c>
       <c r="C77">
-        <v>77.311591878090894</v>
+        <v>77.302140939762296</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>59</v>
@@ -3665,13 +3574,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B78">
-        <v>28.589156773171101</v>
+        <v>28.594221445474702</v>
       </c>
       <c r="C78">
-        <v>77.302140939762296</v>
+        <v>77.294739212602906</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>60</v>
@@ -3695,13 +3604,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B79">
-        <v>28.594221445474702</v>
+        <v>28.604224136350702</v>
       </c>
       <c r="C79">
-        <v>77.294739212602906</v>
+        <v>77.289608238750503</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>61</v>
@@ -3725,13 +3634,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B80">
-        <v>28.604224136350702</v>
+        <v>28.617960082673701</v>
       </c>
       <c r="C80">
-        <v>77.289608238750503</v>
+        <v>77.279377518788905</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>62</v>
@@ -3755,13 +3664,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B81">
-        <v>28.617960082673701</v>
+        <v>28.620549903044001</v>
       </c>
       <c r="C81">
-        <v>77.279377518788905</v>
+        <v>77.249950207612599</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>63</v>
@@ -3785,13 +3694,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B82">
-        <v>28.620549903044001</v>
+        <v>28.6231765741394</v>
       </c>
       <c r="C82">
-        <v>77.249950207612599</v>
+        <v>77.242929487668505</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>64</v>
@@ -3815,13 +3724,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B83">
-        <v>28.6231765741394</v>
+        <v>28.625688812805802</v>
       </c>
       <c r="C83">
-        <v>77.242929487668505</v>
+        <v>77.233759050745405</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>65</v>
@@ -3845,13 +3754,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B84">
-        <v>28.625688812805802</v>
+        <v>28.629940063410501</v>
       </c>
       <c r="C84">
-        <v>77.233759050745405</v>
+        <v>77.224500151890297</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>66</v>
@@ -3875,13 +3784,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="B85">
-        <v>28.629940063410501</v>
+        <v>28.632985106660598</v>
       </c>
       <c r="C85">
-        <v>77.224500151890297</v>
+        <v>77.2193735926963</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>67</v>
@@ -3905,13 +3814,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B86">
-        <v>28.632985106660598</v>
+        <v>28.639239625355</v>
       </c>
       <c r="C86">
-        <v>77.2193735926963</v>
+        <v>77.208558047156799</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>68</v>
@@ -3935,13 +3844,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B87">
-        <v>28.639239625355</v>
+        <v>28.644289665842798</v>
       </c>
       <c r="C87">
-        <v>77.208558047156799</v>
+        <v>77.199922094152797</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>69</v>
@@ -3965,13 +3874,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B88">
-        <v>28.644289665842798</v>
+        <v>28.643985033122199</v>
       </c>
       <c r="C88">
-        <v>77.199922094152797</v>
+        <v>77.188496042332901</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>70</v>
@@ -3995,13 +3904,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B89">
-        <v>28.643985033122199</v>
+        <v>28.642528673360999</v>
       </c>
       <c r="C89">
-        <v>77.188496042332901</v>
+        <v>77.178240252245004</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>71</v>
@@ -4025,13 +3934,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B90">
-        <v>28.642528673360999</v>
+        <v>28.6450299610899</v>
       </c>
       <c r="C90">
-        <v>77.178240252245004</v>
+        <v>77.169270754988702</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>72</v>
@@ -4055,13 +3964,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B91">
-        <v>28.6450299610899</v>
+        <v>28.651620855967899</v>
       </c>
       <c r="C91">
-        <v>77.169270754988702</v>
+        <v>77.158230867122299</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>73</v>
@@ -4085,13 +3994,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B92">
-        <v>28.651620855967899</v>
+        <v>28.655676544109799</v>
       </c>
       <c r="C92">
-        <v>77.158230867122299</v>
+        <v>77.150815272263401</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>74</v>
@@ -4115,13 +4024,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B93">
-        <v>28.655676544109799</v>
+        <v>28.657959448458701</v>
       </c>
       <c r="C93">
-        <v>77.150815272263401</v>
+        <v>77.142668760422296</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>75</v>
@@ -4145,13 +4054,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B94">
-        <v>28.657959448458701</v>
+        <v>28.652750318583301</v>
       </c>
       <c r="C94">
-        <v>77.142668760422296</v>
+        <v>77.131641449311999</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>76</v>
@@ -4175,13 +4084,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B95">
-        <v>28.652750318583301</v>
+        <v>28.643755470130799</v>
       </c>
       <c r="C95">
-        <v>77.131641449311999</v>
+        <v>77.112880009227297</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>43</v>
@@ -4205,13 +4114,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B96">
-        <v>28.643755470130799</v>
+        <v>28.6403902007835</v>
       </c>
       <c r="C96">
-        <v>77.112880009227297</v>
+        <v>77.104952560723405</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>44</v>
@@ -4235,13 +4144,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B97">
-        <v>28.6403902007835</v>
+        <v>28.636568624578601</v>
       </c>
       <c r="C97">
-        <v>77.104952560723405</v>
+        <v>77.096479721920204</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>45</v>
@@ -4265,13 +4174,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B98">
-        <v>28.636568624578601</v>
+        <v>28.633059130156202</v>
       </c>
       <c r="C98">
-        <v>77.096479721920204</v>
+        <v>77.086719375082595</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>46</v>
@@ -4295,13 +4204,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B99">
-        <v>28.633059130156202</v>
+        <v>28.629469757911199</v>
       </c>
       <c r="C99">
-        <v>77.086719375082595</v>
+        <v>77.077769616252496</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>47</v>
@@ -4325,13 +4234,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B100">
-        <v>28.629469757911199</v>
+        <v>28.624802661965202</v>
       </c>
       <c r="C100">
-        <v>77.077769616252496</v>
+        <v>77.0653079835526</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>48</v>
@@ -4355,13 +4264,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B101">
-        <v>28.624802661965202</v>
+        <v>28.621753892048801</v>
       </c>
       <c r="C101">
-        <v>77.0653079835526</v>
+        <v>77.055809982665394</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>49</v>
@@ -4385,13 +4294,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B102">
-        <v>28.621753892048801</v>
+        <v>28.6202603175965</v>
       </c>
       <c r="C102">
-        <v>77.055809982665394</v>
+        <v>77.045068476201294</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>50</v>
@@ -4415,13 +4324,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B103">
-        <v>28.6202603175965</v>
+        <v>28.619292156878</v>
       </c>
       <c r="C103">
-        <v>77.045068476201294</v>
+        <v>77.0333273157202</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>51</v>
@@ -4445,13 +4354,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B104">
-        <v>28.619292156878</v>
+        <v>28.6022201694547</v>
       </c>
       <c r="C104">
-        <v>77.0333273157202</v>
+        <v>77.025940108476703</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>52</v>
@@ -4475,13 +4384,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B105">
-        <v>28.6022201694547</v>
+        <v>28.597199979300601</v>
       </c>
       <c r="C105">
-        <v>77.025940108476703</v>
+        <v>77.033329850863097</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>24</v>
@@ -4505,13 +4414,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B106">
-        <v>28.597199979300601</v>
+        <v>28.592309606260699</v>
       </c>
       <c r="C106">
-        <v>77.033329850863097</v>
+        <v>77.040628011386303</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>53</v>
@@ -4535,13 +4444,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B107">
-        <v>28.592309606260699</v>
+        <v>28.5864966874082</v>
       </c>
       <c r="C107">
-        <v>77.040628011386303</v>
+        <v>77.049473963931604</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>54</v>
@@ -4565,13 +4474,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B108">
-        <v>28.5864966874082</v>
+        <v>28.581124304636301</v>
       </c>
       <c r="C108">
-        <v>77.049473963931604</v>
+        <v>77.057510216573107</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>55</v>
@@ -4595,13 +4504,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B109">
-        <v>28.581124304636301</v>
+        <v>28.574280225021099</v>
       </c>
       <c r="C109">
-        <v>77.057510216573107</v>
+        <v>77.065280259247103</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>56</v>
@@ -4625,13 +4534,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B110">
-        <v>28.574280225021099</v>
+        <v>28.565678011228201</v>
       </c>
       <c r="C110">
-        <v>77.065280259247103</v>
+        <v>77.067103598958496</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>57</v>
@@ -4655,13 +4564,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B111">
-        <v>28.565678011228201</v>
+        <v>28.552206443483499</v>
       </c>
       <c r="C111">
-        <v>77.067103598958496</v>
+        <v>77.058304071046706</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>58</v>
@@ -4684,14 +4593,14 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
-        <v>126</v>
+      <c r="A112" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B112">
-        <v>28.552206443483499</v>
+        <v>28.643720361876198</v>
       </c>
       <c r="C112">
-        <v>77.058304071046706</v>
+        <v>77.222991077753306</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>59</v>
@@ -4715,13 +4624,13 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B113">
-        <v>28.643720361876198</v>
+        <v>28.628770302013798</v>
       </c>
       <c r="C113">
-        <v>77.222991077753306</v>
+        <v>77.211411281736602</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>60</v>
@@ -4745,13 +4654,13 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B114">
-        <v>28.628770302013798</v>
+        <v>28.5918906792391</v>
       </c>
       <c r="C114">
-        <v>77.211411281736602</v>
+        <v>77.161670649185893</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>61</v>
@@ -4775,13 +4684,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B115">
-        <v>28.5918906792391</v>
+        <v>28.548879207757899</v>
       </c>
       <c r="C115">
-        <v>77.161670649185893</v>
+        <v>77.120771046906199</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>62</v>
@@ -4805,13 +4714,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B116">
-        <v>28.548879207757899</v>
+        <v>28.557092193121601</v>
       </c>
       <c r="C116">
-        <v>77.120771046906199</v>
+        <v>77.0868403847564</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>63</v>
@@ -4835,13 +4744,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B117">
-        <v>28.557092193121601</v>
+        <v>28.552205393381598</v>
       </c>
       <c r="C117">
-        <v>77.0868403847564</v>
+        <v>77.058304779260496</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>64</v>
@@ -4864,14 +4773,14 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
-        <v>132</v>
+      <c r="A118" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="B118">
-        <v>28.552205393381598</v>
+        <v>28.662130562366499</v>
       </c>
       <c r="C118">
-        <v>77.058304779260496</v>
+        <v>77.157660899970196</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>65</v>
@@ -4895,13 +4804,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B119">
-        <v>28.662130562366499</v>
+        <v>28.671616181016699</v>
       </c>
       <c r="C119">
-        <v>77.157660899970196</v>
+        <v>77.155225039928098</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>66</v>
@@ -4925,13 +4834,13 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B120">
-        <v>28.671616181016699</v>
+        <v>28.672929594814601</v>
       </c>
       <c r="C120">
-        <v>77.155225039928098</v>
+        <v>77.146059203532801</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>67</v>
@@ -4955,13 +4864,13 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B121">
-        <v>28.672929594814601</v>
+        <v>28.672739521396402</v>
       </c>
       <c r="C121">
-        <v>77.146059203532801</v>
+        <v>77.139179704688601</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>68</v>
@@ -4985,13 +4894,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B122">
-        <v>28.672739521396402</v>
+        <v>28.6749374600302</v>
       </c>
       <c r="C122">
-        <v>77.139179704688601</v>
+        <v>77.130583844176201</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>69</v>
@@ -5015,13 +4924,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B123">
-        <v>28.6749374600302</v>
+        <v>28.676339040177201</v>
       </c>
       <c r="C123">
-        <v>77.130583844176201</v>
+        <v>77.119741306913198</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>70</v>
@@ -5045,13 +4954,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B124">
-        <v>28.676339040177201</v>
+        <v>28.6772690470989</v>
       </c>
       <c r="C124">
-        <v>77.119741306913198</v>
+        <v>77.112410941917204</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>71</v>
@@ -5075,13 +4984,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B125">
-        <v>28.6772690470989</v>
+        <v>28.678601042768101</v>
       </c>
       <c r="C125">
-        <v>77.112410941917204</v>
+        <v>77.102309531720095</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>72</v>
@@ -5105,13 +5014,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B126">
-        <v>28.678601042768101</v>
+        <v>28.679652421819799</v>
       </c>
       <c r="C126">
-        <v>77.102309531720095</v>
+        <v>77.092776962491698</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>73</v>
@@ -5135,13 +5044,13 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B127">
-        <v>28.679652421819799</v>
+        <v>28.681047888529001</v>
       </c>
       <c r="C127">
-        <v>77.092776962491698</v>
+        <v>77.080864811371498</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>74</v>
@@ -5165,13 +5074,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B128">
-        <v>28.681047888529001</v>
+        <v>28.681820552374901</v>
       </c>
       <c r="C128">
-        <v>77.080864811371498</v>
+        <v>77.073958819728702</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>75</v>
@@ -5195,13 +5104,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B129">
-        <v>28.681820552374901</v>
+        <v>28.682330578624398</v>
       </c>
       <c r="C129">
-        <v>77.073958819728702</v>
+        <v>77.064811238709595</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>76</v>
@@ -5225,13 +5134,13 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B130">
-        <v>28.682330578624398</v>
+        <v>28.682133322840698</v>
       </c>
       <c r="C130">
-        <v>77.064811238709595</v>
+        <v>77.056220869321805</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>77</v>
@@ -5255,13 +5164,13 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B131">
-        <v>28.682133322840698</v>
+        <v>28.682279401084902</v>
       </c>
       <c r="C131">
-        <v>77.056220869321805</v>
+        <v>77.044007199850597</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>78</v>
@@ -5285,13 +5194,13 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B132">
-        <v>28.682279401084902</v>
+        <v>28.682390423868899</v>
       </c>
       <c r="C132">
-        <v>77.044007199850597</v>
+        <v>77.030339330316593</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>79</v>
@@ -5315,13 +5224,13 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B133">
-        <v>28.682390423868899</v>
+        <v>28.6834262375694</v>
       </c>
       <c r="C133">
-        <v>77.030339330316593</v>
+        <v>77.017160462350006</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>80</v>
@@ -5345,13 +5254,13 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B134">
-        <v>28.6834262375694</v>
+        <v>28.685237422605798</v>
       </c>
       <c r="C134">
-        <v>77.017160462350006</v>
+        <v>76.996104161659204</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>81</v>
@@ -5375,13 +5284,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B135">
-        <v>28.685237422605798</v>
+        <v>28.6868806432371</v>
       </c>
       <c r="C135">
-        <v>76.996104161659204</v>
+        <v>76.977270141771299</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>82</v>
@@ -5405,13 +5314,13 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B136">
-        <v>28.6868806432371</v>
+        <v>28.688019991474398</v>
       </c>
       <c r="C136">
-        <v>76.977270141771299</v>
+        <v>76.964099063490806</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>83</v>
@@ -5435,13 +5344,13 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B137">
-        <v>28.688019991474398</v>
+        <v>28.6892409043414</v>
       </c>
       <c r="C137">
-        <v>76.964099063490806</v>
+        <v>76.951146665673804</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>84</v>
@@ -5465,13 +5374,13 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B138">
-        <v>28.6892409043414</v>
+        <v>28.690739832981301</v>
       </c>
       <c r="C138">
-        <v>76.951146665673804</v>
+        <v>76.935379165790494</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>85</v>
@@ -5495,13 +5404,13 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B139">
-        <v>28.690739832981301</v>
+        <v>28.697409334400302</v>
       </c>
       <c r="C139">
-        <v>76.935379165790494</v>
+        <v>76.919270891978201</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>86</v>
@@ -5524,14 +5433,14 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A140" s="5" t="s">
-        <v>154</v>
+      <c r="A140" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="B140">
-        <v>28.697409334400302</v>
+        <v>28.6233297481776</v>
       </c>
       <c r="C140">
-        <v>76.919270891978201</v>
+        <v>77.267919640441406</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>87</v>
@@ -5555,13 +5464,13 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="B141">
-        <v>28.6233297481776</v>
+        <v>28.630679432771299</v>
       </c>
       <c r="C141">
-        <v>77.267919640441406</v>
+        <v>77.277620312446004</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>88</v>
@@ -5585,13 +5494,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B142">
-        <v>28.630679432771299</v>
+        <v>28.636629548609001</v>
       </c>
       <c r="C142">
-        <v>77.277620312446004</v>
+        <v>77.286830185019397</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>89</v>
@@ -5615,13 +5524,13 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B143">
-        <v>28.636629548609001</v>
+        <v>28.6417092412096</v>
       </c>
       <c r="C143">
-        <v>77.286830185019397</v>
+        <v>77.295430104275297</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>90</v>
@@ -5645,13 +5554,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B144">
-        <v>28.6417092412096</v>
+        <v>28.648490927029201</v>
       </c>
       <c r="C144">
-        <v>77.295430104275297</v>
+        <v>77.305580443624194</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>91</v>
@@ -5675,13 +5584,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B145">
-        <v>28.648490927029201</v>
+        <v>28.6469535188082</v>
       </c>
       <c r="C145">
-        <v>77.305580443624194</v>
+        <v>77.315914564594706</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>92</v>
@@ -5705,13 +5614,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B146">
-        <v>28.6469535188082</v>
+        <v>28.645481854355999</v>
       </c>
       <c r="C146">
-        <v>77.315914564594706</v>
+        <v>77.324360455161099</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>93</v>
@@ -5735,13 +5644,13 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B147">
-        <v>28.645481854355999</v>
+        <v>28.6498397665314</v>
       </c>
       <c r="C147">
-        <v>77.324360455161099</v>
+        <v>77.339680435649896</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>94</v>
@@ -5764,14 +5673,14 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>161</v>
+      <c r="A148" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="B148">
-        <v>28.6498397665314</v>
+        <v>28.656855046855298</v>
       </c>
       <c r="C148">
-        <v>77.339680435649896</v>
+        <v>77.236811500252003</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>95</v>
@@ -5795,13 +5704,13 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B149">
-        <v>28.656855046855298</v>
+        <v>28.649550154223899</v>
       </c>
       <c r="C149">
-        <v>77.236811500252003</v>
+        <v>77.238020475375507</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>96</v>
@@ -5825,13 +5734,13 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B150">
-        <v>28.649550154223899</v>
+        <v>28.6400787453825</v>
       </c>
       <c r="C150">
-        <v>77.238020475375507</v>
+        <v>77.240510337156095</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>97</v>
@@ -5855,13 +5764,13 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B151">
-        <v>28.6400787453825</v>
+        <v>28.6283900472928</v>
       </c>
       <c r="C151">
-        <v>77.240510337156095</v>
+        <v>77.241180497270605</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>98</v>
@@ -5885,13 +5794,13 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B152">
-        <v>28.6283900472928</v>
+        <v>28.625059274534699</v>
       </c>
       <c r="C152">
-        <v>77.241180497270605</v>
+        <v>77.219186035839897</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>56</v>
@@ -5915,13 +5824,13 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B153">
-        <v>28.625059274534699</v>
+        <v>28.6021528203323</v>
       </c>
       <c r="C153">
-        <v>77.219186035839897</v>
+        <v>77.229019098919693</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>99</v>
@@ -5945,13 +5854,13 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B154">
-        <v>28.6021528203323</v>
+        <v>28.589361412844099</v>
       </c>
       <c r="C154">
-        <v>77.229019098919693</v>
+        <v>77.233562311572399</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>100</v>
@@ -5975,13 +5884,13 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B155">
-        <v>28.589361412844099</v>
+        <v>28.583310106945</v>
       </c>
       <c r="C155">
-        <v>77.233562311572399</v>
+        <v>77.239659478788397</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>101</v>
@@ -6005,13 +5914,13 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B156">
-        <v>28.583310106945</v>
+        <v>28.56401304273</v>
       </c>
       <c r="C156">
-        <v>77.239659478788397</v>
+        <v>77.234244842207502</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>102</v>
@@ -6035,13 +5944,13 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B157">
-        <v>28.56401304273</v>
+        <v>28.555386570871601</v>
       </c>
       <c r="C157">
-        <v>77.234244842207502</v>
+        <v>77.241954775686807</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>103</v>
@@ -6065,13 +5974,13 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B158">
-        <v>28.555386570871601</v>
+        <v>28.551402794891199</v>
       </c>
       <c r="C158">
-        <v>77.241954775686807</v>
+        <v>77.251765547569704</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>104</v>
@@ -6095,13 +6004,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B159">
-        <v>28.551402794891199</v>
+        <v>28.5443980877813</v>
       </c>
       <c r="C159">
-        <v>77.251765547569704</v>
+        <v>77.264350887547806</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>105</v>
@@ -6125,13 +6034,13 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B160">
-        <v>28.5443980877813</v>
+        <v>28.5429211710495</v>
       </c>
       <c r="C160">
-        <v>77.264350887547806</v>
+        <v>77.275039134540293</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>106</v>
@@ -6155,13 +6064,13 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B161">
-        <v>28.5429211710495</v>
+        <v>28.538129918547899</v>
       </c>
       <c r="C161">
-        <v>77.275039134540293</v>
+        <v>77.283300269850798</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>107</v>
@@ -6185,13 +6094,13 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B162">
-        <v>28.538129918547899</v>
+        <v>28.528729799210801</v>
       </c>
       <c r="C162">
-        <v>77.283300269850798</v>
+        <v>77.288219957303497</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>108</v>
@@ -6215,13 +6124,13 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B163">
-        <v>28.528729799210801</v>
+        <v>28.519520178670501</v>
       </c>
       <c r="C163">
-        <v>77.288219957303497</v>
+        <v>77.294561275071999</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>109</v>
@@ -6245,13 +6154,13 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B164">
-        <v>28.519520178670501</v>
+        <v>28.5025396916053</v>
       </c>
       <c r="C164">
-        <v>77.294561275071999</v>
+        <v>77.299300379445498</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>110</v>
@@ -6275,13 +6184,13 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B165">
-        <v>28.5025396916053</v>
+        <v>28.4932481926256</v>
       </c>
       <c r="C165">
-        <v>77.299300379445498</v>
+        <v>77.302970201886794</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>111</v>
@@ -6305,13 +6214,13 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B166">
-        <v>28.4932481926256</v>
+        <v>28.478069719434</v>
       </c>
       <c r="C166">
-        <v>77.302970201886794</v>
+        <v>77.304899543916093</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>112</v>
@@ -6335,13 +6244,13 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B167">
-        <v>28.478069719434</v>
+        <v>28.457701052176699</v>
       </c>
       <c r="C167">
-        <v>77.304899543916093</v>
+        <v>77.307442449950301</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>113</v>
@@ -6365,13 +6274,13 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B168">
-        <v>28.457701052176699</v>
+        <v>28.448566699781001</v>
       </c>
       <c r="C168">
-        <v>77.307442449950301</v>
+        <v>77.308053953337904</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>114</v>
@@ -6395,13 +6304,13 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B169">
-        <v>28.448566699781001</v>
+        <v>28.4380097428886</v>
       </c>
       <c r="C169">
-        <v>77.308053953337904</v>
+        <v>77.308990581401503</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>115</v>
@@ -6425,13 +6334,13 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B170">
-        <v>28.4380097428886</v>
+        <v>28.422753372562799</v>
       </c>
       <c r="C170">
-        <v>77.308990581401503</v>
+        <v>77.310357510441705</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>116</v>
@@ -6455,13 +6364,13 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B171">
-        <v>28.422753372562799</v>
+        <v>28.4107709763285</v>
       </c>
       <c r="C171">
-        <v>77.310357510441705</v>
+        <v>77.311506870205704</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>117</v>
@@ -6485,13 +6394,13 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B172">
-        <v>28.4107709763285</v>
+        <v>28.3976672686073</v>
       </c>
       <c r="C172">
-        <v>77.311506870205704</v>
+        <v>77.312365745611999</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>118</v>
@@ -6515,13 +6424,13 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B173">
-        <v>28.3976672686073</v>
+        <v>28.385988653548999</v>
       </c>
       <c r="C173">
-        <v>77.312365745611999</v>
+        <v>77.313420553715005</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>119</v>
@@ -6545,13 +6454,13 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B174">
-        <v>28.385988653548999</v>
+        <v>28.370159590446502</v>
       </c>
       <c r="C174">
-        <v>77.313420553715005</v>
+        <v>77.314940323286507</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>120</v>
@@ -6575,13 +6484,13 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B175">
-        <v>28.370159590446502</v>
+        <v>28.354672735977001</v>
       </c>
       <c r="C175">
-        <v>77.314940323286507</v>
+        <v>77.316218987572597</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>121</v>
@@ -6605,13 +6514,13 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B176">
-        <v>28.354672735977001</v>
+        <v>28.339801287463999</v>
       </c>
       <c r="C176">
-        <v>77.316218987572597</v>
+        <v>77.316446234849096</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>122</v>
@@ -6634,14 +6543,14 @@
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A177" s="6" t="s">
-        <v>192</v>
+      <c r="A177" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="B177">
-        <v>28.339801287463999</v>
+        <v>28.629469921823301</v>
       </c>
       <c r="C177">
-        <v>77.316446234849096</v>
+        <v>77.0777690378155</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>123</v>
@@ -6665,13 +6574,13 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B178">
-        <v>28.629469921823301</v>
+        <v>28.615903596054402</v>
       </c>
       <c r="C178">
-        <v>77.0777690378155</v>
+        <v>77.085257352505195</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>124</v>
@@ -6695,13 +6604,13 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B179">
-        <v>28.615903596054402</v>
+        <v>28.602349160543699</v>
       </c>
       <c r="C179">
-        <v>77.085257352505195</v>
+        <v>77.082540780412003</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>125</v>
@@ -6725,13 +6634,13 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B180">
-        <v>28.602349160543699</v>
+        <v>28.589068987330499</v>
       </c>
       <c r="C180">
-        <v>77.082540780412003</v>
+        <v>77.082959337262807</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>79</v>
@@ -6755,13 +6664,13 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B181">
-        <v>28.589068987330499</v>
+        <v>28.577110092991301</v>
       </c>
       <c r="C181">
-        <v>77.082959337262807</v>
+        <v>77.111300145604801</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>80</v>
@@ -6785,13 +6694,13 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B182">
-        <v>28.577110092991301</v>
+        <v>28.565298856604102</v>
       </c>
       <c r="C182">
-        <v>77.111300145604801</v>
+        <v>77.122380223283599</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>81</v>
@@ -6815,13 +6724,13 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B183">
-        <v>28.565298856604102</v>
+        <v>28.560813098146301</v>
       </c>
       <c r="C183">
-        <v>77.122380223283599</v>
+        <v>77.140345119389707</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>82</v>
@@ -6845,13 +6754,13 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B184">
-        <v>28.560813098146301</v>
+        <v>28.557829391908498</v>
       </c>
       <c r="C184">
-        <v>77.140345119389707</v>
+        <v>77.160990976941306</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>83</v>
@@ -6875,13 +6784,13 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B185">
-        <v>28.557829391908498</v>
+        <v>28.5578921824175</v>
       </c>
       <c r="C185">
-        <v>77.160990976941306</v>
+        <v>77.1739692727852</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>84</v>
@@ -6905,13 +6814,13 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B186">
-        <v>28.5578921824175</v>
+        <v>28.5503479810769</v>
       </c>
       <c r="C186">
-        <v>77.1739692727852</v>
+        <v>77.185147594707402</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>85</v>
@@ -6935,13 +6844,13 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B187">
-        <v>28.5503479810769</v>
+        <v>28.547199587198701</v>
       </c>
       <c r="C187">
-        <v>77.185147594707402</v>
+        <v>77.193817402223203</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>86</v>
@@ -6965,13 +6874,13 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B188">
-        <v>28.547199587198701</v>
+        <v>28.5423379050509</v>
       </c>
       <c r="C188">
-        <v>77.193817402223203</v>
+        <v>77.220508311316493</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>87</v>
@@ -6995,13 +6904,13 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B189">
-        <v>28.5423379050509</v>
+        <v>28.541229104353</v>
       </c>
       <c r="C189">
-        <v>77.220508311316493</v>
+        <v>77.229381924649601</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>88</v>
@@ -7025,13 +6934,13 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B190">
-        <v>28.541229104353</v>
+        <v>28.541831639041298</v>
       </c>
       <c r="C190">
-        <v>77.229381924649601</v>
+        <v>77.238248363896403</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>89</v>
@@ -7055,13 +6964,13 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B191">
-        <v>28.541831639041298</v>
+        <v>28.545851298999999</v>
       </c>
       <c r="C191">
-        <v>77.238248363896403</v>
+        <v>77.251167888477994</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>90</v>
@@ -7085,13 +6994,13 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="B192">
-        <v>28.545851298999999</v>
+        <v>28.549448648028601</v>
       </c>
       <c r="C192">
-        <v>77.251167888477994</v>
+        <v>77.259220451360207</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>91</v>
@@ -7115,13 +7024,13 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="B193">
-        <v>28.549448648028601</v>
+        <v>28.5544251656586</v>
       </c>
       <c r="C193">
-        <v>77.259220451360207</v>
+        <v>77.264884225102605</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>92</v>
@@ -7145,13 +7054,13 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B194">
-        <v>28.5544251656586</v>
+        <v>28.559774777569899</v>
       </c>
       <c r="C194">
-        <v>77.264884225102605</v>
+        <v>77.275126684787395</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>93</v>
@@ -7175,13 +7084,13 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B195">
-        <v>28.559774777569899</v>
+        <v>28.5629492801487</v>
       </c>
       <c r="C195">
-        <v>77.275126684787395</v>
+        <v>77.286220013057701</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>94</v>
@@ -7205,13 +7114,13 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B196">
-        <v>28.5629492801487</v>
+        <v>28.561089095012399</v>
       </c>
       <c r="C196">
-        <v>77.286220013057701</v>
+        <v>77.291890219025106</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>95</v>
@@ -7235,13 +7144,13 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B197">
-        <v>28.561089095012399</v>
+        <v>28.545978516428399</v>
       </c>
       <c r="C197">
-        <v>77.291890219025106</v>
+        <v>77.296648171073102</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>96</v>
@@ -7265,13 +7174,13 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B198">
-        <v>28.545978516428399</v>
+        <v>28.542834687771499</v>
       </c>
       <c r="C198">
-        <v>77.296648171073102</v>
+        <v>77.310176122803696</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>97</v>
@@ -7295,13 +7204,13 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B199">
-        <v>28.542834687771499</v>
+        <v>28.552862322747099</v>
       </c>
       <c r="C199">
-        <v>77.310176122803696</v>
+        <v>77.321651224969798</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>98</v>
@@ -7324,14 +7233,14 @@
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A200" s="7" t="s">
-        <v>214</v>
+      <c r="A200" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="B200">
-        <v>28.552862322747099</v>
+        <v>28.721613473524801</v>
       </c>
       <c r="C200">
-        <v>77.321651224969798</v>
+        <v>77.289493759556393</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>56</v>
@@ -7355,13 +7264,13 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B201">
-        <v>28.721613473524801</v>
+        <v>28.713180821817101</v>
       </c>
       <c r="C201">
-        <v>77.289493759556393</v>
+        <v>77.290060393714299</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>99</v>
@@ -7385,13 +7294,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B202">
-        <v>28.713180821817101</v>
+        <v>28.702409627163401</v>
       </c>
       <c r="C202">
-        <v>77.290060393714299</v>
+        <v>77.285979944577505</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>100</v>
@@ -7415,13 +7324,13 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" s="8" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="B203">
-        <v>28.702409627163401</v>
+        <v>28.692102704718501</v>
       </c>
       <c r="C203">
-        <v>77.285979944577505</v>
+        <v>77.279611805001096</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>101</v>
@@ -7445,13 +7354,13 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="8" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="B204">
-        <v>28.692102704718501</v>
+        <v>28.682757940643</v>
       </c>
       <c r="C204">
-        <v>77.279611805001096</v>
+        <v>77.274747925911498</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>102</v>
@@ -7475,13 +7384,13 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B205">
-        <v>28.682757940643</v>
+        <v>28.664789263425199</v>
       </c>
       <c r="C205">
-        <v>77.274747925911498</v>
+        <v>77.284799516904798</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>103</v>
@@ -7505,13 +7414,13 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B206">
-        <v>28.664789263425199</v>
+        <v>28.658039111388</v>
       </c>
       <c r="C206">
-        <v>77.284799516904798</v>
+        <v>77.290030957244895</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>104</v>
@@ -7535,13 +7444,13 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B207">
-        <v>28.658039111388</v>
+        <v>28.6535882873339</v>
       </c>
       <c r="C207">
-        <v>77.290030957244895</v>
+        <v>77.295589290013496</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>105</v>
@@ -7565,13 +7474,13 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B208">
-        <v>28.6535882873339</v>
+        <v>28.6484903117755</v>
       </c>
       <c r="C208">
-        <v>77.295589290013496</v>
+        <v>77.305579946048098</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>106</v>
@@ -7595,13 +7504,13 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B209">
-        <v>28.6484903117755</v>
+        <v>28.631934962036802</v>
       </c>
       <c r="C209">
-        <v>77.305579946048098</v>
+        <v>77.310758168767194</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>107</v>
@@ -7625,13 +7534,13 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B210">
-        <v>28.631934962036802</v>
+        <v>28.624877238436699</v>
       </c>
       <c r="C210">
-        <v>77.310758168767194</v>
+        <v>77.304373069171703</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>108</v>
@@ -7655,13 +7564,13 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B211">
-        <v>28.624877238436699</v>
+        <v>28.620056382275401</v>
       </c>
       <c r="C211">
-        <v>77.304373069171703</v>
+        <v>77.305271078311904</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>109</v>
@@ -7685,13 +7594,13 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B212">
-        <v>28.620056382275401</v>
+        <v>28.613588930403601</v>
       </c>
       <c r="C212">
-        <v>77.305271078311904</v>
+        <v>77.308839187919702</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>110</v>
@@ -7715,13 +7624,13 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B213">
-        <v>28.613588930403601</v>
+        <v>28.605793597260799</v>
       </c>
       <c r="C213">
-        <v>77.308839187919702</v>
+        <v>77.298703718584804</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>111</v>
@@ -7745,13 +7654,13 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" s="8" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="B214">
-        <v>28.605793597260799</v>
+        <v>28.604226021226999</v>
       </c>
       <c r="C214">
-        <v>77.298703718584804</v>
+        <v>77.289609195602793</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>112</v>
@@ -7775,13 +7684,13 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" s="8" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="B215">
-        <v>28.604226021226999</v>
+        <v>28.589359088063901</v>
       </c>
       <c r="C215">
-        <v>77.289609195602793</v>
+        <v>77.257130659049196</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>113</v>
@@ -7805,13 +7714,13 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="8" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="B216">
-        <v>28.589359088063901</v>
+        <v>28.572163808779099</v>
       </c>
       <c r="C216">
-        <v>77.257130659049196</v>
+        <v>77.258510436393294</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>114</v>
@@ -7835,13 +7744,13 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B217">
-        <v>28.572163808779099</v>
+        <v>28.565943512492201</v>
       </c>
       <c r="C217">
-        <v>77.258510436393294</v>
+        <v>77.250500445360103</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>115</v>
@@ -7865,13 +7774,13 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" s="8" t="s">
-        <v>218</v>
+        <v>170</v>
       </c>
       <c r="B218">
-        <v>28.565943512492201</v>
+        <v>28.570557014911</v>
       </c>
       <c r="C218">
-        <v>77.250500445360103</v>
+        <v>77.236450540505899</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>116</v>
@@ -7895,13 +7804,13 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" s="8" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="B219">
-        <v>28.570557014911</v>
+        <v>28.568608756246601</v>
       </c>
       <c r="C219">
-        <v>77.236450540505899</v>
+        <v>77.220265959474204</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>117</v>
@@ -7925,13 +7834,13 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B220">
-        <v>28.568608756246601</v>
+        <v>28.574448036879399</v>
       </c>
       <c r="C220">
-        <v>77.220265959474204</v>
+        <v>77.209622014560395</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>118</v>
@@ -7955,13 +7864,13 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B221">
-        <v>28.574448036879399</v>
+        <v>28.5758067143584</v>
       </c>
       <c r="C221">
-        <v>77.209622014560395</v>
+        <v>77.198571662873206</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>119</v>
@@ -7985,13 +7894,13 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B222">
-        <v>28.5758067143584</v>
+        <v>28.570210100240601</v>
       </c>
       <c r="C222">
-        <v>77.198571662873206</v>
+        <v>77.187888168719695</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>120</v>
@@ -8015,13 +7924,13 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B223">
-        <v>28.570210100240601</v>
+        <v>28.578503232375098</v>
       </c>
       <c r="C223">
-        <v>77.187888168719695</v>
+        <v>77.175724913223803</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>121</v>
@@ -8045,13 +7954,13 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B224">
-        <v>28.578503232375098</v>
+        <v>28.589379212162701</v>
       </c>
       <c r="C224">
-        <v>77.175724913223803</v>
+        <v>77.169518459722298</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>122</v>
@@ -8075,13 +7984,13 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B225">
-        <v>28.589379212162701</v>
+        <v>28.6087783604228</v>
       </c>
       <c r="C225">
-        <v>77.169518459722298</v>
+        <v>77.140340309977503</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>123</v>
@@ -8105,13 +8014,13 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B226">
-        <v>28.6087783604228</v>
+        <v>28.6241247739203</v>
       </c>
       <c r="C226">
-        <v>77.140340309977503</v>
+        <v>77.136489735532905</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>124</v>
@@ -8135,13 +8044,13 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B227">
-        <v>28.6241247739203</v>
+        <v>28.6370978386072</v>
       </c>
       <c r="C227">
-        <v>77.136489735532905</v>
+        <v>77.129741999686004</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>125</v>
@@ -8165,13 +8074,13 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" s="8" t="s">
-        <v>227</v>
+        <v>108</v>
       </c>
       <c r="B228">
-        <v>28.6370978386072</v>
+        <v>28.649017630375202</v>
       </c>
       <c r="C228">
-        <v>77.129741999686004</v>
+        <v>77.122708003357999</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>126</v>
@@ -8195,13 +8104,13 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" s="8" t="s">
-        <v>108</v>
+        <v>228</v>
       </c>
       <c r="B229">
-        <v>28.649017630375202</v>
+        <v>28.658159612364798</v>
       </c>
       <c r="C229">
-        <v>77.122708003357999</v>
+        <v>77.127320771564101</v>
       </c>
       <c r="D229" s="4" t="s">
         <v>127</v>
@@ -8225,13 +8134,13 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B230">
-        <v>28.658159612364798</v>
+        <v>28.6857797103671</v>
       </c>
       <c r="C230">
-        <v>77.127320771564101</v>
+        <v>77.149627094061799</v>
       </c>
       <c r="D230" s="4" t="s">
         <v>128</v>
@@ -8255,13 +8164,13 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B231">
-        <v>28.6857797103671</v>
+        <v>28.701818716562901</v>
       </c>
       <c r="C231">
-        <v>77.149627094061799</v>
+        <v>77.165191000128303</v>
       </c>
       <c r="D231" s="4" t="s">
         <v>129</v>
@@ -8285,13 +8194,13 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" s="8" t="s">
-        <v>230</v>
+        <v>47</v>
       </c>
       <c r="B232">
-        <v>28.701818716562901</v>
+        <v>28.7070207026944</v>
       </c>
       <c r="C232">
-        <v>77.165191000128303</v>
+        <v>77.180520146902097</v>
       </c>
       <c r="D232" s="4" t="s">
         <v>130</v>
@@ -8315,13 +8224,13 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" s="8" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="B233">
-        <v>28.7070207026944</v>
+        <v>28.724159068637199</v>
       </c>
       <c r="C233">
-        <v>77.180520146902097</v>
+        <v>77.182049745323894</v>
       </c>
       <c r="D233" s="4" t="s">
         <v>131</v>
@@ -8344,14 +8253,14 @@
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A234" s="8" t="s">
-        <v>231</v>
+      <c r="A234" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="B234">
-        <v>28.724159068637199</v>
+        <v>28.6149213991858</v>
       </c>
       <c r="C234">
-        <v>77.182049745323894</v>
+        <v>77.022719507362694</v>
       </c>
       <c r="D234" s="4" t="s">
         <v>128</v>
@@ -8375,13 +8284,13 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="9" t="s">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="B235">
-        <v>28.6149213991858</v>
+        <v>28.6172393372767</v>
       </c>
       <c r="C235">
-        <v>77.022719507362694</v>
+        <v>77.010401277784396</v>
       </c>
       <c r="D235" s="4" t="s">
         <v>129</v>
@@ -8405,13 +8314,13 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B236">
-        <v>28.6172393372767</v>
+        <v>28.612676316443899</v>
       </c>
       <c r="C236">
-        <v>77.010401277784396</v>
+        <v>76.986543061126397</v>
       </c>
       <c r="D236" s="4" t="s">
         <v>130</v>
@@ -8435,13 +8344,13 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B237">
-        <v>28.612676316443899</v>
+        <v>28.611899028160099</v>
       </c>
       <c r="C237">
-        <v>76.986543061126397</v>
+        <v>76.978001469249307</v>
       </c>
       <c r="D237" s="4" t="s">
         <v>131</v>
@@ -8464,15 +8373,6 @@
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A238" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="B238">
-        <v>28.611899028160099</v>
-      </c>
-      <c r="C238">
-        <v>76.978001469249307</v>
-      </c>
       <c r="D238" s="4" t="s">
         <v>132</v>
       </c>

</xml_diff>